<commit_message>
added project risk register
</commit_message>
<xml_diff>
--- a/Deliverables.xlsx
+++ b/Deliverables.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Capstone\Administration\Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\university work\Year 4\Master Projects\Administration\Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B448C7-6D2E-42A1-B309-9CE63D3BFC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA8834-96EB-4F05-918D-EBF5BB637D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA57EB97-12E4-48A3-8EAF-7FD1826F846C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{DA57EB97-12E4-48A3-8EAF-7FD1826F846C}"/>
   </bookViews>
   <sheets>
     <sheet name="Milestones" sheetId="1" r:id="rId1"/>
     <sheet name="Milestones at risk" sheetId="2" r:id="rId2"/>
+    <sheet name="Risk Register" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
   <si>
     <t>Description</t>
   </si>
@@ -274,22 +275,77 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID </t>
+  </si>
+  <si>
+    <t>Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probability </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mitigation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date raised </t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Contingency plan</t>
+  </si>
+  <si>
+    <t>Risk Description</t>
+  </si>
+  <si>
+    <t>Illness of team member</t>
+  </si>
+  <si>
+    <t>Mentor weekly inavailability</t>
+  </si>
+  <si>
+    <t>Team member timetable clash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part Manufacturing error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed off by </t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Project files save Corruption/overwrite</t>
+  </si>
+  <si>
+    <t>Have muliple backups of main repository</t>
+  </si>
+  <si>
+    <t>Team member Injury</t>
+  </si>
+  <si>
+    <t>don’t be clumsy you silly bitch</t>
+  </si>
+  <si>
+    <t>HHTC room avialability</t>
+  </si>
+  <si>
+    <t>3D Printing Availability</t>
+  </si>
+  <si>
+    <t>Get required 3D printing CAD drawings completed early</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -311,19 +367,19 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7F7F7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -333,30 +389,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDCDCDC"/>
+        <fgColor rgb="FFDAE9F8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5F9FD"/>
+        <fgColor rgb="FFD9D9D9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0F0F0"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -387,17 +455,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -407,101 +464,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -510,25 +479,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -540,22 +494,22 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -567,28 +521,96 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -598,135 +620,135 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,6 +757,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDAE9F8"/>
+      <color rgb="FFD9D9D9"/>
+      <color rgb="FFF2F2F2"/>
       <color rgb="FFF0F0F0"/>
       <color rgb="FFF5F9FD"/>
       <color rgb="FFD3D3D3"/>
@@ -1073,526 +1098,526 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB687DE-7B59-445C-B2C7-8E146C5C6618}">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.875" customWidth="1"/>
-    <col min="2" max="2" width="7.25" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="50.875" customWidth="1"/>
-    <col min="5" max="6" width="16.125" customWidth="1"/>
-    <col min="7" max="9" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="9" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1"/>
-    <row r="2" spans="2:9" s="1" customFormat="1" ht="35.1" customHeight="1" thickBot="1">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" s="1" customFormat="1" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B3" s="13">
+    <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B4" s="13">
+      <c r="H3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
         <v>1.2</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="28" t="s">
+      <c r="H4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B6" s="13">
+      <c r="H5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="22"/>
+    </row>
+    <row r="6" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
         <v>1.3</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="29" t="s">
+      <c r="H6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B8" s="30" t="s">
+      <c r="H7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B9" s="31" t="s">
+      <c r="H8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B10" s="13">
+      <c r="H9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
         <v>2.1</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B11" s="13">
+      <c r="H10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B12" s="13">
+      <c r="H11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B13" s="29" t="s">
+      <c r="H12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B14" s="30" t="s">
+      <c r="H13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B15" s="40" t="s">
+      <c r="H14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1">
-      <c r="B16" s="41" t="s">
+      <c r="H15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B17" s="31" t="s">
+      <c r="H16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B18" s="13">
+      <c r="H17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7">
         <v>3.1</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B19" s="13">
+      <c r="H18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7">
         <v>3.2</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="16"/>
-    </row>
-    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B20" s="13">
+      <c r="H19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
         <v>3.3</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="16"/>
-    </row>
-    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B21" s="39" t="s">
+      <c r="H20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B22" s="42">
+      <c r="H21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="16"/>
+      <c r="H22" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1604,124 +1629,356 @@
   <dimension ref="B4:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
-    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="15" thickBot="1"/>
-    <row r="5" spans="2:6" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B5" s="46" t="s">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15">
-      <c r="B6" s="49" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="52"/>
-    </row>
-    <row r="7" spans="2:6" ht="15">
-      <c r="B7" s="53" t="s">
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="54"/>
-    </row>
-    <row r="8" spans="2:6" ht="15">
-      <c r="B8" s="53" t="s">
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="54"/>
-    </row>
-    <row r="9" spans="2:6" ht="15">
-      <c r="B9" s="53" t="s">
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="54"/>
-    </row>
-    <row r="10" spans="2:6" ht="15">
-      <c r="B10" s="53" t="s">
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="54"/>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B11" s="55" t="s">
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="59"/>
+      <c r="F11" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B009BBA-9CF0-42B9-8B30-C2F0D833DC46}">
+  <dimension ref="B2:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" customWidth="1"/>
+    <col min="9" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:11" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="45">
+        <v>45576</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="5">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+      <c r="G4" s="48">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="48">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="46">
+        <v>45576</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>2</v>
+      </c>
+      <c r="G6" s="49">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="46">
+        <v>45576</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="49">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="46">
+        <v>45576</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8</v>
+      </c>
+      <c r="G8" s="50">
+        <v>48</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="46">
+        <v>45576</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="4">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>10</v>
+      </c>
+      <c r="G9" s="51">
+        <v>40</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6</v>
+      </c>
+      <c r="G10" s="51">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="4">
+        <v>8</v>
+      </c>
+      <c r="F11" s="4">
+        <v>4</v>
+      </c>
+      <c r="G11" s="51">
+        <v>32</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>